<commit_message>
commit before i start removing not import stuff
</commit_message>
<xml_diff>
--- a/Excel/Copy of Tables of results v4.xlsx
+++ b/Excel/Copy of Tables of results v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Uni\FINAL_Year\Dissertation\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90CFFE5-9443-428D-8305-5AAA3C7C01D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB0DA23-5905-455C-A3A4-61073ED0EAFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{A522EAAA-04A2-4FA9-A435-DE8F63DB9FA3}"/>
+    <workbookView xWindow="7200" yWindow="795" windowWidth="21600" windowHeight="11385" xr2:uid="{A522EAAA-04A2-4FA9-A435-DE8F63DB9FA3}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="2" r:id="rId1"/>
@@ -33466,8 +33466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938C8F6B-38BB-4F78-8766-277B22481226}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38527,7 +38527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FA0EB7-1895-4D82-91BB-779D518BA066}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>

</xml_diff>